<commit_message>
Added ability of adding new bills in user form and finished method of receipt's generating
</commit_message>
<xml_diff>
--- a/src/resources/receipts/out_receipt.xlsx
+++ b/src/resources/receipts/out_receipt.xlsx
@@ -246,7 +246,7 @@
     <t>14:00, Сб, вс выходной)</t>
   </si>
   <si>
-    <t>г. Москва, ул. Пролетарская, д. 15, кв. 5</t>
+    <t>г. Иркутск, ул. Лермонтова, д. 10, кв. 1</t>
   </si>
   <si>
     <t>Июнь 2021</t>
@@ -255,10 +255,10 @@
     <t>31.06.2021г.</t>
   </si>
   <si>
-    <t>14.06.2021г.</t>
-  </si>
-  <si>
-    <t>Астафьев Владимир Дмитриевич</t>
+    <t>15.06.2021г.</t>
+  </si>
+  <si>
+    <t>Иванов Иван Иванович</t>
   </si>
 </sst>
 </file>
@@ -2194,11 +2194,11 @@
       <c r="C35" s="16"/>
       <c r="D35" s="17"/>
       <c r="E35" s="114" t="n">
-        <v>1200.0</v>
+        <v>450.0</v>
       </c>
       <c r="F35" s="115"/>
       <c r="G35" s="114" t="n">
-        <v>1500.0</v>
+        <v>600.0</v>
       </c>
       <c r="H35" s="115"/>
       <c r="I35" s="114">

</xml_diff>

<commit_message>
Add edit login and password function
</commit_message>
<xml_diff>
--- a/src/resources/receipts/out_receipt.xlsx
+++ b/src/resources/receipts/out_receipt.xlsx
@@ -246,7 +246,7 @@
     <t>14:00, Сб, вс выходной)</t>
   </si>
   <si>
-    <t>г. Иркутск, ул. Лермонтова, д. 10, кв. 1</t>
+    <t>г. Москва, ул. Пролетарская, д. 15, кв. 5</t>
   </si>
   <si>
     <t>Июнь 2021</t>
@@ -255,10 +255,10 @@
     <t>31.06.2021г.</t>
   </si>
   <si>
-    <t>15.06.2021г.</t>
-  </si>
-  <si>
-    <t>Иванов Иван Иванович</t>
+    <t>16.06.2021г.</t>
+  </si>
+  <si>
+    <t>Астафьев Владимир Дмитриевич</t>
   </si>
 </sst>
 </file>
@@ -2194,11 +2194,11 @@
       <c r="C35" s="16"/>
       <c r="D35" s="17"/>
       <c r="E35" s="114" t="n">
-        <v>450.0</v>
+        <v>200.0</v>
       </c>
       <c r="F35" s="115"/>
       <c r="G35" s="114" t="n">
-        <v>600.0</v>
+        <v>202.0</v>
       </c>
       <c r="H35" s="115"/>
       <c r="I35" s="114">

</xml_diff>